<commit_message>
Updated the input parameters into the presets.
</commit_message>
<xml_diff>
--- a/C5V_outputs/output.xlsx
+++ b/C5V_outputs/output.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
   <si>
     <t>Input Values</t>
   </si>
@@ -48,7 +48,7 @@
     <t>Middle-Aged (United States)</t>
   </si>
   <si>
-    <t>C-type: A Bit Peaked</t>
+    <t>B-type: Somewhat Broad</t>
   </si>
   <si>
     <t>Total Number Hospitalized</t>
@@ -69,10 +69,10 @@
     <t>Severe Scenario</t>
   </si>
   <si>
-    <t>205,804</t>
-  </si>
-  <si>
-    <t>314,854</t>
+    <t>48,395</t>
+  </si>
+  <si>
+    <t>472,281</t>
   </si>
   <si>
     <t>Total Number Admitted</t>
@@ -108,106 +108,112 @@
     <t>Pediatric ICU Cases</t>
   </si>
   <si>
-    <t>189,979</t>
-  </si>
-  <si>
-    <t>10,495</t>
-  </si>
-  <si>
-    <t>5,330</t>
+    <t>38,412</t>
+  </si>
+  <si>
+    <t>9,603</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>1,757</t>
+  </si>
+  <si>
+    <t>439</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>12,651</t>
+  </si>
+  <si>
+    <t>3,731</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>13,444</t>
+  </si>
+  <si>
+    <t>5,282</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>5,626</t>
-  </si>
-  <si>
-    <t>311</t>
-  </si>
-  <si>
-    <t>158</t>
-  </si>
-  <si>
-    <t>61</t>
+    <t>24,968</t>
+  </si>
+  <si>
+    <t>4,321</t>
+  </si>
+  <si>
+    <t>395,669</t>
+  </si>
+  <si>
+    <t>64,120</t>
+  </si>
+  <si>
+    <t>12,492</t>
+  </si>
+  <si>
+    <t>18,101</t>
+  </si>
+  <si>
+    <t>2,933</t>
+  </si>
+  <si>
+    <t>571</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>36,685</t>
-  </si>
-  <si>
-    <t>4,810</t>
-  </si>
-  <si>
-    <t>707</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>9,499</t>
-  </si>
-  <si>
-    <t>2,624</t>
-  </si>
-  <si>
-    <t>180,480</t>
-  </si>
-  <si>
-    <t>7,871</t>
-  </si>
-  <si>
-    <t>5,329</t>
-  </si>
-  <si>
-    <t>263,780</t>
-  </si>
-  <si>
-    <t>42,746</t>
-  </si>
-  <si>
-    <t>8,328</t>
-  </si>
-  <si>
-    <t>7,811</t>
-  </si>
-  <si>
-    <t>1,266</t>
-  </si>
-  <si>
-    <t>247</t>
-  </si>
-  <si>
-    <t>50,935</t>
-  </si>
-  <si>
-    <t>19,593</t>
-  </si>
-  <si>
-    <t>1,104</t>
-  </si>
-  <si>
-    <t>13,189</t>
-  </si>
-  <si>
-    <t>10,687</t>
-  </si>
-  <si>
-    <t>250,591</t>
-  </si>
-  <si>
-    <t>32,060</t>
-  </si>
-  <si>
-    <t>8,327</t>
+    <t>130,318</t>
+  </si>
+  <si>
+    <t>24,914</t>
+  </si>
+  <si>
+    <t>2,542</t>
+  </si>
+  <si>
+    <t>138,484</t>
+  </si>
+  <si>
+    <t>35,266</t>
+  </si>
+  <si>
+    <t>257,185</t>
+  </si>
+  <si>
+    <t>28,854</t>
+  </si>
+  <si>
+    <t>12,491</t>
   </si>
   <si>
     <t>Total Medical Ward Patients</t>
@@ -222,10 +228,10 @@
     <t>Total Patient-Days for COVID Ward Patients</t>
   </si>
   <si>
-    <t>1,253,862</t>
-  </si>
-  <si>
-    <t>1,740,945</t>
+    <t>288,091</t>
+  </si>
+  <si>
+    <t>2,967,520</t>
   </si>
   <si>
     <t>Total ICU Patients</t>
@@ -240,16 +246,16 @@
     <t>Peak Ventilator Need (80% Ventilated Fraction)</t>
   </si>
   <si>
-    <t>181,039</t>
-  </si>
-  <si>
-    <t>737,377</t>
-  </si>
-  <si>
-    <t>3,848</t>
-  </si>
-  <si>
-    <t>15,674</t>
+    <t>86,427</t>
+  </si>
+  <si>
+    <t>577,077</t>
+  </si>
+  <si>
+    <t>2,985</t>
+  </si>
+  <si>
+    <t>19,931</t>
   </si>
 </sst>
 </file>
@@ -750,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -766,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -774,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -790,7 +796,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -829,13 +835,13 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>102.1</v>
+        <v>2.4</v>
       </c>
       <c r="D2">
-        <v>5.9</v>
+        <v>38.7</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -846,13 +852,13 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>156.2</v>
+        <v>23.4</v>
       </c>
       <c r="D3">
-        <v>7.6</v>
+        <v>36.8</v>
       </c>
       <c r="E3">
-        <v>11.8</v>
+        <v>8.6</v>
       </c>
     </row>
   </sheetData>
@@ -902,19 +908,19 @@
         <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -928,7 +934,7 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>39</v>
@@ -937,10 +943,10 @@
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -954,7 +960,7 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>40</v>
@@ -963,10 +969,10 @@
         <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -977,19 +983,19 @@
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -1036,25 +1042,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1062,25 +1068,25 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1088,25 +1094,25 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
         <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1114,25 +1120,25 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1150,16 +1156,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1173,10 +1179,10 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1184,16 +1190,16 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1211,19 +1217,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1240,10 +1246,10 @@
         <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1251,19 +1257,19 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>